<commit_message>
mistake corrected: participant that wanted to be removed after prenotification is now indicated as bounce, so the numbers in this table remain correct.
</commit_message>
<xml_diff>
--- a/sample_descriptives.xlsx
+++ b/sample_descriptives.xlsx
@@ -1,98 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tilburgu-my.sharepoint.com/personal/a_bouma_tilburguniversity_edu/Documents/Documents/PhD/1. Survey Project/Simulation_Questionnaire/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F23E5121EC89E2BBCE6733BF073E1B939259F601" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{488324EA-C60C-402A-8A67-180B22204AF5}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>Source.Title</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>included</t>
-  </si>
-  <si>
-    <t>percentage</t>
-  </si>
-  <si>
-    <t>delivered_invitations</t>
-  </si>
-  <si>
-    <t>ADVANCES IN METHODS AND PRACTICES IN PSYCHOLOGICAL SCIENCE</t>
-  </si>
-  <si>
-    <t>APPLIED MEASUREMENT IN EDUCATION</t>
-  </si>
-  <si>
-    <t>APPLIED PSYCHOLOGICAL MEASUREMENT</t>
-  </si>
-  <si>
-    <t>BEHAVIOR RESEARCH METHODS</t>
-  </si>
-  <si>
-    <t>BRITISH JOURNAL OF MATHEMATICAL &amp; STATISTICAL PSYCHOLOGY</t>
-  </si>
-  <si>
-    <t>EDUCATIONAL AND PSYCHOLOGICAL MEASUREMENT</t>
-  </si>
-  <si>
-    <t>EDUCATIONAL MEASUREMENT-ISSUES AND PRACTICE</t>
-  </si>
-  <si>
-    <t>JOURNAL OF CLASSIFICATION</t>
-  </si>
-  <si>
-    <t>JOURNAL OF EDUCATIONAL AND BEHAVIORAL STATISTICS</t>
-  </si>
-  <si>
-    <t>JOURNAL OF EDUCATIONAL MEASUREMENT</t>
-  </si>
-  <si>
-    <t>JOURNAL OF MATHEMATICAL PSYCHOLOGY</t>
-  </si>
-  <si>
-    <t>JOURNAL OF MEASUREMENT AND EVALUATION IN EDUCATION AND PSYCHOLOGY-EPOD</t>
-  </si>
-  <si>
-    <t>METHODOLOGY-EUROPEAN JOURNAL OF RESEARCH METHODS FOR THE BEHAVIORAL AND SOCIAL SCIENCES</t>
-  </si>
-  <si>
-    <t>MULTIVARIATE BEHAVIORAL RESEARCH</t>
-  </si>
-  <si>
-    <t>ORGANIZATIONAL RESEARCH METHODS</t>
-  </si>
-  <si>
-    <t>PSYCHOLOGICAL METHODS</t>
-  </si>
-  <si>
-    <t>PSYCHOMETRIKA</t>
+    <t xml:space="preserve">Source.Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delivered_invitations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVANCES IN METHODS AND PRACTICES IN PSYCHOLOGICAL SCIENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLIED MEASUREMENT IN EDUCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLIED PSYCHOLOGICAL MEASUREMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEHAVIOR RESEARCH METHODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRITISH JOURNAL OF MATHEMATICAL &amp; STATISTICAL PSYCHOLOGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATIONAL AND PSYCHOLOGICAL MEASUREMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATIONAL MEASUREMENT-ISSUES AND PRACTICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOURNAL OF CLASSIFICATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOURNAL OF EDUCATIONAL AND BEHAVIORAL STATISTICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOURNAL OF EDUCATIONAL MEASUREMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOURNAL OF MATHEMATICAL PSYCHOLOGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOURNAL OF MEASUREMENT AND EVALUATION IN EDUCATION AND PSYCHOLOGY-EPOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METHODOLOGY-EUROPEAN JOURNAL OF RESEARCH METHODS FOR THE BEHAVIORAL AND SOCIAL SCIENCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTIVARIATE BEHAVIORAL RESEARCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZATIONAL RESEARCH METHODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSYCHOLOGICAL METHODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSYCHOMETRIKA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,15 +121,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -418,19 +402,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="97.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,297 +426,297 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>84</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>11</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>50</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>28</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>52</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>37</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>71</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>756</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>154</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>90</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>70</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>78</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>115</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>71</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>62</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>112</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>9</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>8</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>74</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>42</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>57</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>102</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>71</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>70</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>73</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>48</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>66</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>76</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>12</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>16</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>51</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>10</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>20</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>27</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>17</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>63</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>169</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>114</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>67</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>71</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>12</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>17</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>282</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>171</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>61</v>
       </c>
-      <c r="E17">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>140</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>88</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>63</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>